<commit_message>
test for multiple sheets
</commit_message>
<xml_diff>
--- a/src/test/resources/files/test_populated_template.xlsx
+++ b/src/test/resources/files/test_populated_template.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Sheet 1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Test Sheet 2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Test Key 1</t>
   </si>
@@ -38,6 +39,15 @@
   </si>
   <si>
     <t xml:space="preserve">Test Value 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random Key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random Key 2</t>
   </si>
 </sst>
 </file>
@@ -140,7 +150,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -182,4 +192,50 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="C6:D9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
first very rough implementation of type checking
</commit_message>
<xml_diff>
--- a/src/test/resources/files/test_populated_template.xlsx
+++ b/src/test/resources/files/test_populated_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Test Sheet 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -148,10 +148,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -183,6 +183,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -201,14 +209,14 @@
   </sheetPr>
   <dimension ref="C6:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.27"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>

</xml_diff>

<commit_message>
test passing! datastructure capturing cell values and types from a spreadsheet
</commit_message>
<xml_diff>
--- a/src/test/resources/files/test_populated_template.xlsx
+++ b/src/test/resources/files/test_populated_template.xlsx
@@ -148,10 +148,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -190,6 +190,9 @@
       <c r="B10" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="C10" s="0" t="n">
+        <v>12.1</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -210,7 +213,7 @@
   <dimension ref="C6:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
test passing: checking for types in parsed spreadsheet
</commit_message>
<xml_diff>
--- a/src/test/resources/files/test_populated_template.xlsx
+++ b/src/test/resources/files/test_populated_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Test Key 1</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t xml:space="preserve">Test Value 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formula Result</t>
   </si>
   <si>
     <t xml:space="preserve">Random Key</t>
@@ -148,15 +151,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -192,6 +197,25 @@
       </c>
       <c r="C10" s="0" t="n">
         <v>12.1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="n">
+        <v>1234.55</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="n">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <f aca="false">SUM(C10:C12)</f>
+        <v>1436.65</v>
       </c>
     </row>
   </sheetData>
@@ -226,15 +250,15 @@
   <sheetData>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>234</v>

</xml_diff>

<commit_message>
failing test - checking for forumla that returns string
</commit_message>
<xml_diff>
--- a/src/test/resources/files/test_populated_template.xlsx
+++ b/src/test/resources/files/test_populated_template.xlsx
@@ -151,10 +151,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -216,6 +216,12 @@
       <c r="C13" s="0" t="n">
         <f aca="false">SUM(C10:C12)</f>
         <v>1436.65</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0" t="str">
+        <f aca="false">B13</f>
+        <v>Formula Result</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing for date values in cells
</commit_message>
<xml_diff>
--- a/src/test/resources/files/test_populated_template.xlsx
+++ b/src/test/resources/files/test_populated_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Sheet 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Test Key 1</t>
   </si>
@@ -51,14 +51,19 @@
   </si>
   <si>
     <t xml:space="preserve">Random Key 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="166" formatCode="D\ MMM\ YYYY"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -125,12 +130,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -153,7 +166,7 @@
   </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -240,10 +253,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C6:D9"/>
+  <dimension ref="C6:D11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -270,6 +283,19 @@
         <v>234</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>51920</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D11" s="3" t="n">
+        <v>43466</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
This is what previous commit was meant to be.
</commit_message>
<xml_diff>
--- a/src/test/resources/files/test_populated_template.xlsx
+++ b/src/test/resources/files/test_populated_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Sheet 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -180,8 +180,8 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -227,7 +227,7 @@
       <c r="D7" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="3" t="n">
         <v>43575</v>
       </c>
     </row>
@@ -235,7 +235,7 @@
       <c r="D8" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="3" t="n">
         <v>43579</v>
       </c>
     </row>
@@ -291,10 +291,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C6:D11"/>
+  <dimension ref="C6:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -320,12 +320,15 @@
       <c r="D9" s="0" t="n">
         <v>234</v>
       </c>
+      <c r="E9" s="0" t="n">
+        <v>234</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="2" t="n">
         <v>51920</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Part-way through implementing first test of Datamapline rules
</commit_message>
<xml_diff>
--- a/src/test/resources/files/test_populated_template.xlsx
+++ b/src/test/resources/files/test_populated_template.xlsx
@@ -69,11 +69,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="167" formatCode="D\ MMM\ YYYY"/>
+    <numFmt numFmtId="166" formatCode="D\ MMM\ YYYY"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -140,7 +139,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -154,10 +153,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -227,7 +222,7 @@
       <c r="D7" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="2" t="n">
         <v>43575</v>
       </c>
     </row>
@@ -235,7 +230,7 @@
       <c r="D8" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="2" t="n">
         <v>43579</v>
       </c>
     </row>
@@ -321,7 +316,7 @@
         <v>234</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -333,7 +328,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="4" t="n">
+      <c r="D11" s="3" t="n">
         <v>43466</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Failing test - but first working stab at Rule checking
</commit_message>
<xml_diff>
--- a/src/test/resources/files/test_populated_template.xlsx
+++ b/src/test/resources/files/test_populated_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Test Key 1</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compare Val 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compare Val 2</t>
   </si>
 </sst>
 </file>
@@ -286,10 +292,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C6:E11"/>
+  <dimension ref="C6:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -332,6 +338,22 @@
         <v>43466</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
very tenuous - ruleset test for greater than passes, but very fragile
</commit_message>
<xml_diff>
--- a/src/test/resources/files/test_populated_template.xlsx
+++ b/src/test/resources/files/test_populated_template.xlsx
@@ -295,7 +295,7 @@
   <dimension ref="C6:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -319,10 +319,10 @@
         <v>12</v>
       </c>
       <c r="D9" s="0" t="n">
+        <v>235</v>
+      </c>
+      <c r="E9" s="0" t="n">
         <v>234</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>235</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added less than rule checker
</commit_message>
<xml_diff>
--- a/src/test/resources/files/test_populated_template.xlsx
+++ b/src/test/resources/files/test_populated_template.xlsx
@@ -292,10 +292,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C6:E15"/>
+  <dimension ref="C6:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -354,6 +354,14 @@
         <v>230</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>